<commit_message>
merged in LP fix 3.19 ready for IB 1 and for Jessica ABF work
</commit_message>
<xml_diff>
--- a/state_program_statistics/Actual Leave Data 2012-2016_CZ.xlsx
+++ b/state_program_statistics/Actual Leave Data 2012-2016_CZ.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workfiles\Microsimulation\microsim\data\state_program_statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workfiles\Microsimulation\microsim\state_program_statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C94637A-5F60-498B-B0B1-8E4E22957E50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC3F64E-14E1-46F0-966C-05AA7C9567D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6930" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="4" r:id="rId1"/>
     <sheet name="California" sheetId="1" r:id="rId2"/>
     <sheet name="New Jersey" sheetId="2" r:id="rId3"/>
     <sheet name="Rhode Island" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="IB 1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="109">
   <si>
     <t>Participated for own illness leave</t>
   </si>
@@ -325,6 +325,45 @@
   </si>
   <si>
     <t>inflation adjusted to 2012 dollars</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>2012-2016</t>
+  </si>
+  <si>
+    <t>Exhibit 1 (total outlay)</t>
+  </si>
+  <si>
+    <t>Exhibit 3 (CA participants by leave type)</t>
+  </si>
+  <si>
+    <t>bond</t>
+  </si>
+  <si>
+    <t>illchild</t>
+  </si>
+  <si>
+    <t>illspouse</t>
+  </si>
+  <si>
+    <t>illparent</t>
+  </si>
+  <si>
+    <t>Exhibit 4 (NJ participants by leave type)</t>
+  </si>
+  <si>
+    <t>Exhibit 5 (RI participants by leave type)</t>
   </si>
 </sst>
 </file>
@@ -343,7 +382,7 @@
     <numFmt numFmtId="168" formatCode="#,##0.0000"/>
     <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,6 +409,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -416,6 +456,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -500,7 +546,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -556,6 +602,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="169" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -602,6 +653,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -887,28 +942,28 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A42" sqref="A42:XFD42"/>
+      <selection pane="topRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1328125" customWidth="1"/>
+    <col min="12" max="12" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.86328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -934,7 +989,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -969,7 +1024,7 @@
         <v>12988555.560000001</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1004,7 +1059,7 @@
         <v>12988555.560000001</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1039,7 +1094,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1074,7 +1129,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1109,7 +1164,7 @@
         <v>3778</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1144,7 +1199,7 @@
         <v>204.66666666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1179,7 +1234,7 @@
         <v>565.66666666666663</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1214,7 +1269,7 @@
         <v>345.33333333333331</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1241,7 +1296,7 @@
         <v>44893.666666666664</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1264,7 +1319,7 @@
         <v>164915.79999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1291,7 +1346,7 @@
         <v>6.7042154650228558E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1314,7 +1369,7 @@
         <v>5530</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1337,7 +1392,7 @@
         <v>8928</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1360,7 +1415,7 @@
         <v>8901</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1383,7 +1438,7 @@
         <v>4564995820.8000002</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1406,7 +1461,7 @@
         <v>604813176.39999998</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1429,7 +1484,7 @@
         <v>5169808997.1999998</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="42" t="s">
         <v>95</v>
       </c>
@@ -1441,7 +1496,7 @@
       <c r="J19" s="46"/>
       <c r="L19" s="47"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" s="49" t="s">
         <v>9</v>
       </c>
@@ -1455,7 +1510,7 @@
       <c r="J20" s="46"/>
       <c r="L20" s="47"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" s="49" t="s">
         <v>10</v>
       </c>
@@ -1469,7 +1524,7 @@
       <c r="J21" s="46"/>
       <c r="L21" s="47"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" s="49" t="s">
         <v>11</v>
       </c>
@@ -1483,17 +1538,17 @@
       <c r="J22" s="46"/>
       <c r="L22" s="47"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
         <v>18</v>
       </c>
@@ -1502,7 +1557,7 @@
         <v>366.66666666666669</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="8" t="s">
         <v>19</v>
       </c>
@@ -1511,22 +1566,22 @@
         <v>366.66666666666669</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A29" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A30" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>45</v>
       </c>
@@ -1534,7 +1589,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
         <v>39</v>
       </c>
@@ -1584,7 +1639,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A37" s="26">
         <v>12</v>
       </c>
@@ -1644,7 +1699,7 @@
         <v>8970.1731938506036</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A38" s="26">
         <v>13</v>
       </c>
@@ -1704,7 +1759,7 @@
         <v>8681.3010281054521</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A39" s="26">
         <v>14</v>
       </c>
@@ -1764,7 +1819,7 @@
         <v>8583.3539932844669</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A40" s="26">
         <v>15</v>
       </c>
@@ -1824,7 +1879,7 @@
         <v>8959.0533133034914</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A41" s="26">
         <v>16</v>
       </c>
@@ -1884,7 +1939,7 @@
         <v>9311.3772286576732</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A42" s="26"/>
       <c r="B42" s="2">
         <f>AVERAGE(B37:B41)</f>
@@ -1931,7 +1986,7 @@
         <v>8901.0517514403364</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A43" s="26"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1943,7 +1998,7 @@
       <c r="M43" s="28"/>
       <c r="N43" s="2"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A44" s="26"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1976,17 +2031,17 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="A10" sqref="A10:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="57.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="15.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>15</v>
       </c>
@@ -2006,7 +2061,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2022,7 +2077,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2034,7 +2089,7 @@
         <v>17282000</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2043,11 +2098,11 @@
         <v>3.273680933919685E-2</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F9" si="1">F10/F$3</f>
+        <f>F10/F$3</f>
         <v>3.273680933919685E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -2056,11 +2111,11 @@
         <v>4.0418073718319642E-3</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F4:F9" si="1">F11/F$3</f>
         <v>4.0418073718319642E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -2073,7 +2128,7 @@
         <v>2.578311150329823E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -2086,7 +2141,7 @@
         <v>3.9694167920379594E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2099,7 +2154,7 @@
         <v>9.7343478764031939E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2112,7 +2167,7 @@
         <v>1.2065096632334221E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2141,7 +2196,7 @@
         <v>573758.995</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2165,7 +2220,7 @@
         <v>74030.883000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -2189,7 +2244,7 @@
         <v>44431.540500000003</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2213,7 +2268,7 @@
         <v>71342.005000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2237,7 +2292,7 @@
         <v>172994</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2264,7 +2319,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -2294,7 +2349,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -2329,7 +2384,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -2364,7 +2419,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -2394,7 +2449,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -2424,7 +2479,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -2460,22 +2515,22 @@
         <v>1082.2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
         <v>37</v>
       </c>
@@ -2493,20 +2548,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="96.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="96.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>15</v>
       </c>
@@ -2535,7 +2590,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2551,7 +2606,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2563,7 +2618,7 @@
         <v>3831200</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2576,7 +2631,7 @@
         <v>1.7494518688661517E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -2589,7 +2644,7 @@
         <v>3.7716642305282938E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -2602,7 +2657,7 @@
         <v>2.7850281896011692E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -2615,7 +2670,7 @@
         <v>4.8861975360200462E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2628,7 +2683,7 @@
         <v>6.3003758613489249E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2641,7 +2696,7 @@
         <v>6.597932762580915E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2669,7 +2724,7 @@
         <v>64209</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2700,7 +2755,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -2731,7 +2786,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2762,7 +2817,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2793,7 +2848,7 @@
       </c>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2823,7 +2878,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>90</v>
       </c>
@@ -2853,7 +2908,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -2883,7 +2938,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -2894,7 +2949,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -2927,7 +2982,7 @@
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -2960,12 +3015,12 @@
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(C21:G21)</f>
         <v>506940000</v>
       </c>
       <c r="C21" s="3">
@@ -2992,33 +3047,33 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>17</v>
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="F30" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E31">
         <v>2012</v>
       </c>
@@ -3026,7 +3081,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E32">
         <v>2013</v>
       </c>
@@ -3034,7 +3089,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="33" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:17" x14ac:dyDescent="0.45">
       <c r="E33">
         <v>2014</v>
       </c>
@@ -3042,7 +3097,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="34" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:17" x14ac:dyDescent="0.45">
       <c r="E34">
         <v>2015</v>
       </c>
@@ -3050,7 +3105,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="35" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:17" x14ac:dyDescent="0.45">
       <c r="E35">
         <v>2016</v>
       </c>
@@ -3058,7 +3113,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="36" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:17" x14ac:dyDescent="0.45">
       <c r="E36" t="s">
         <v>91</v>
       </c>
@@ -3087,20 +3142,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="57.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -3114,7 +3169,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -3130,7 +3185,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -3143,7 +3198,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -3156,7 +3211,7 @@
         <v>7.0402409638554223E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -3169,7 +3224,7 @@
         <v>1.4120481927710844E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -3182,7 +3237,7 @@
         <v>4.8192771084337347E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -3195,7 +3250,7 @@
         <v>8.1927710843373496E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -3208,7 +3263,7 @@
         <v>2.3467469879518071E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -3221,7 +3276,7 @@
         <v>9.1638554216867465E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -3242,7 +3297,7 @@
         <v>31097.25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -3260,7 +3315,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -3278,7 +3333,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -3296,7 +3351,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -3317,7 +3372,7 @@
         <v>10365.75</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -3335,7 +3390,7 @@
         <v>4684</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -3353,7 +3408,7 @@
         <v>41463</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -3374,7 +3429,7 @@
         <v>5882</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -3395,7 +3450,7 @@
         <v>47345</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -3416,7 +3471,7 @@
         <v>160575104</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -3434,7 +3489,7 @@
         <v>11201050</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -3452,22 +3507,22 @@
         <v>171776154</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C25" s="40" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="33" t="s">
         <v>57</v>
       </c>
@@ -3488,7 +3543,7 @@
         <v>229.6</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="34"/>
       <c r="B27" s="35" t="s">
         <v>14</v>
@@ -3509,7 +3564,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="34" t="s">
         <v>59</v>
       </c>
@@ -3527,7 +3582,7 @@
         <v>39680</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="34" t="s">
         <v>58</v>
       </c>
@@ -3545,7 +3600,7 @@
         <v>3870</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="34" t="s">
         <v>61</v>
       </c>
@@ -3563,7 +3618,7 @@
         <v>2847</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="34" t="s">
         <v>62</v>
       </c>
@@ -3581,7 +3636,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="34" t="s">
         <v>60</v>
       </c>
@@ -3599,7 +3654,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="34" t="s">
         <v>63</v>
       </c>
@@ -3617,7 +3672,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="34" t="s">
         <v>64</v>
       </c>
@@ -3638,7 +3693,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" s="34" t="s">
         <v>65</v>
       </c>
@@ -3659,7 +3714,7 @@
         <v>35810</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" s="34" t="s">
         <v>75</v>
       </c>
@@ -3671,7 +3726,7 @@
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" s="34" t="s">
         <v>76</v>
       </c>
@@ -3683,7 +3738,7 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="34" t="s">
         <v>66</v>
       </c>
@@ -3691,7 +3746,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" s="34" t="s">
         <v>68</v>
       </c>
@@ -3712,7 +3767,7 @@
         <v>446.77111724032881</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="34" t="s">
         <v>70</v>
       </c>
@@ -3730,7 +3785,7 @@
         <v>367638</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" s="34" t="s">
         <v>72</v>
       </c>
@@ -3748,7 +3803,7 @@
         <v>164250040</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="34" t="s">
         <v>69</v>
       </c>
@@ -3769,7 +3824,7 @@
         <v>473.94166043380704</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="34" t="s">
         <v>71</v>
       </c>
@@ -3787,7 +3842,7 @@
         <v>13370</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="34" t="s">
         <v>73</v>
       </c>
@@ -3805,7 +3860,7 @@
         <v>6336600</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="34" t="s">
         <v>74</v>
       </c>
@@ -3826,12 +3881,12 @@
         <v>170586640</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" s="43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" s="41" t="s">
         <v>68</v>
       </c>
@@ -3852,7 +3907,7 @@
         <v>433.36987122255812</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="34" t="s">
         <v>70</v>
       </c>
@@ -3870,7 +3925,7 @@
         <v>367638</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="41" t="s">
         <v>72</v>
       </c>
@@ -3891,7 +3946,7 @@
         <v>159323232.71651879</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="41" t="s">
         <v>69</v>
       </c>
@@ -3912,7 +3967,7 @@
         <v>459.72541290917655</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="34" t="s">
         <v>71</v>
       </c>
@@ -3930,7 +3985,7 @@
         <v>13370</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="41" t="s">
         <v>73</v>
       </c>
@@ -3951,7 +4006,7 @@
         <v>6146528.7705956912</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="41" t="s">
         <v>74</v>
       </c>
@@ -3972,12 +4027,12 @@
         <v>165469761.48711449</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -4012,12 +4067,248 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D82DAC-6301-4138-9431-4FB81094A8CB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="33.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.46484375" style="51" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B2" s="52" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="53">
+        <v>5169808997.1999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="54">
+        <v>506940000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="53">
+        <v>169506472.65396079</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B6" s="53"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B8" s="55" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="53">
+        <v>568461.23379999993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="53">
+        <v>164915.79999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="53">
+        <v>199723.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="53">
+        <v>41997.542560000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="53">
+        <v>67797.255199999985</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="53">
+        <v>67550.566200000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B15" s="55"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B17" s="55" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="53">
+        <v>68691.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="53">
+        <v>24112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="53">
+        <v>25262.666666666668</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="53">
+        <v>1127.6666666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="53">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="53">
+        <v>1976.3333333333333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B24" s="55"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B26" s="55" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="53">
+        <v>26351.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="53">
+        <v>8783.8333333333339</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="53">
+        <v>3778</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="53">
+        <v>204.66666666666666</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" s="53">
+        <v>553.66666666666663</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" s="53">
+        <v>331.66666666666669</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed clf_mord bug for chunk2 states, pow X 1 for state of work=False
</commit_message>
<xml_diff>
--- a/state_program_statistics/Actual Leave Data 2012-2016_CZ.xlsx
+++ b/state_program_statistics/Actual Leave Data 2012-2016_CZ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workfiles\Microsimulation\microsim\state_program_statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC3F64E-14E1-46F0-966C-05AA7C9567D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF4BF6A-B211-439A-8C0C-E679438E992B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6930" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="4" r:id="rId1"/>
@@ -546,7 +546,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -607,6 +607,7 @@
     <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -653,10 +654,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -941,8 +938,8 @@
   <dimension ref="A1:T44"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C18" sqref="C18"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1169,7 +1166,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="13">
-        <v>2.578311150329823E-3</v>
+        <v>2.57831115032982E-3</v>
       </c>
       <c r="C7" s="13">
         <v>3.5002088118605136E-4</v>
@@ -1179,7 +1176,7 @@
       </c>
       <c r="E7" s="14">
         <f>AVERAGE(Table1[[#This Row],[California]:[Rhode Island]])</f>
-        <v>1.1367532474530827E-3</v>
+        <v>1.1367532474530816E-3</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23">
@@ -2030,8 +2027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2093,9 +2090,9 @@
       <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="11">
-        <f t="shared" si="0"/>
-        <v>3.273680933919685E-2</v>
+      <c r="B4" s="56">
+        <f>B10/$B$2</f>
+        <v>3.2893255051498663E-2</v>
       </c>
       <c r="F4">
         <f>F10/F$3</f>
@@ -2106,12 +2103,12 @@
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="11">
-        <f t="shared" si="0"/>
-        <v>4.0418073718319642E-3</v>
+      <c r="B5" s="56">
+        <f>B11/$B$2</f>
+        <v>3.9229982177988653E-3</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F4:F9" si="1">F11/F$3</f>
+        <f t="shared" ref="F5:F9" si="1">F11/F$3</f>
         <v>4.0418073718319642E-3</v>
       </c>
     </row>
@@ -2119,9 +2116,9 @@
       <c r="A6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="11">
-        <f t="shared" si="0"/>
-        <v>2.578311150329823E-3</v>
+      <c r="B6" s="56">
+        <f>B12/$B$2</f>
+        <v>2.4301320773058676E-3</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
@@ -2132,9 +2129,9 @@
       <c r="A7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="11">
-        <f t="shared" si="0"/>
-        <v>3.9694167920379594E-3</v>
+      <c r="B7" s="56">
+        <f>B13/$B$2</f>
+        <v>3.9087238861242914E-3</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
@@ -2145,9 +2142,9 @@
       <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="11">
-        <f t="shared" si="0"/>
-        <v>9.7343478764031939E-3</v>
+      <c r="B8" s="56">
+        <f>B14/$B$2</f>
+        <v>9.5426339544034244E-3</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
@@ -2158,9 +2155,9 @@
       <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="11">
-        <f t="shared" si="0"/>
-        <v>1.2065096632334221E-2</v>
+      <c r="B9" s="56">
+        <f>B15/$B$2</f>
+        <v>1.1556717972456892E-2</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
@@ -2171,7 +2168,7 @@
       <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="30">
         <f t="shared" si="0"/>
         <v>568461.23379999993</v>
       </c>
@@ -2200,8 +2197,8 @@
       <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="2">
-        <f t="shared" ref="B11:B21" si="2">AVERAGE(C11:G11)</f>
+      <c r="B11" s="30">
+        <f>AVERAGE(C11:G11)</f>
         <v>67797.255199999985</v>
       </c>
       <c r="C11" s="5">
@@ -2224,8 +2221,8 @@
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="2">
-        <f t="shared" si="2"/>
+      <c r="B12" s="30">
+        <f t="shared" ref="B11:B21" si="2">AVERAGE(C12:G12)</f>
         <v>41997.542560000002</v>
       </c>
       <c r="C12" s="5">
@@ -2248,7 +2245,7 @@
       <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="30">
         <f t="shared" si="2"/>
         <v>67550.566200000001</v>
       </c>
@@ -2272,7 +2269,7 @@
       <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="30">
         <f t="shared" si="2"/>
         <v>164915.79999999999</v>
       </c>
@@ -2296,7 +2293,7 @@
       <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="30">
         <f t="shared" si="2"/>
         <v>199723.2</v>
       </c>
@@ -2791,7 +2788,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="39">
-        <f t="shared" ref="B13:B21" si="2">AVERAGE(C13:G13)</f>
+        <f t="shared" ref="B13:B20" si="2">AVERAGE(C13:G13)</f>
         <v>1976.3333333333333</v>
       </c>
       <c r="C13" s="16"/>
@@ -4069,7 +4066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D82DAC-6301-4138-9431-4FB81094A8CB}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>

</xml_diff>